<commit_message>
updates to functionality all pages exist
</commit_message>
<xml_diff>
--- a/content/individual topics.xlsx
+++ b/content/individual topics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\Functional skills site newbuild\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C07468-9093-4F9E-A95F-0E29BE130833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7F08C3-D2C7-4620-AB33-59E13B131165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="1965" windowWidth="19095" windowHeight="7005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="1965" windowWidth="19095" windowHeight="10590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>topic</t>
   </si>
@@ -43,6 +43,51 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/PGc33iLXaTE</t>
+  </si>
+  <si>
+    <t>subtracting</t>
+  </si>
+  <si>
+    <t>multiplying</t>
+  </si>
+  <si>
+    <t>decimals</t>
+  </si>
+  <si>
+    <t>fractions</t>
+  </si>
+  <si>
+    <t>fdp</t>
+  </si>
+  <si>
+    <t>percentages</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -371,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -408,7 +453,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -419,7 +464,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -430,7 +475,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -441,7 +486,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -452,7 +497,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -463,12 +508,111 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -481,6 +625,7 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{FBF738C9-CD57-4A14-AA9F-4D6ACB39586F}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{45CCA532-7268-4468-9158-5A6CC755E75A}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{F9616E41-A359-4B4D-96E5-9EC0054003F8}"/>
+    <hyperlink ref="B9:B17" r:id="rId8" display="https://www.youtube.com/embed/PGc33iLXaTE" xr:uid="{1630DC0A-0697-491C-9748-2E3FA1C5DB0C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>